<commit_message>
Change frequency sorting, improve scaling, clean up code,  make disabling attributes work via headers, swap frquency and value to fit cells, fix bugs
</commit_message>
<xml_diff>
--- a/test_data/test_data_short_1.xlsx
+++ b/test_data/test_data_short_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\source\BP\GroupGen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\source\BP\GroupGen\GroupGen\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEEB895-D2A3-482F-B421-8C77BC42FC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D1893A-C534-42B7-8BE3-4DE9A0317341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{37D1C687-089E-486E-A61D-B2B374414689}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37D1C687-089E-486E-A61D-B2B374414689}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
   <si>
     <t>Christoph</t>
   </si>
@@ -474,12 +474,12 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -493,7 +493,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,7 +507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -521,7 +521,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -535,7 +535,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -549,7 +549,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -563,7 +563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -577,7 +577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -591,7 +591,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -605,7 +605,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -619,7 +619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -633,7 +633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -647,7 +647,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -661,7 +661,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -675,7 +675,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -689,7 +689,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -703,21 +703,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
       <c r="D17">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -731,7 +728,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>